<commit_message>
Updated the update records into the database algorithm
</commit_message>
<xml_diff>
--- a/dummy_data/Cleaned Animal data.xlsx
+++ b/dummy_data/Cleaned Animal data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CEMA PROJECTS\animalHealthSurveillance\animal-surveillance\pipelines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CEMA PROJECTS\animalHealthSurveillance\animal-surveillance\dummy_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C97FFCF-50CD-468C-8FCA-92AC6104C8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216C3E34-CE3A-45DD-A7B9-031DDBC6980F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1603,7 +1603,7 @@
   <dimension ref="A1:Y501"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>